<commit_message>
adding item in backlog
</commit_message>
<xml_diff>
--- a/SSW695/product backlog.xlsx.xlsx
+++ b/SSW695/product backlog.xlsx.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stevens data\3rd SEM\SSW_Capstone\SSW695_Team7\SSW695\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SSW-695\SSW695_Team7\SSW695\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="28800" windowHeight="16536" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="product backlog" sheetId="5" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="63">
   <si>
     <t>User Story</t>
   </si>
@@ -211,9 +211,6 @@
     <t>In progress</t>
   </si>
   <si>
-    <t>Pranay, Sonali, Akshay</t>
-  </si>
-  <si>
     <t>Testing Login, Registration API calls with SQLITE db on localhost with Postman</t>
   </si>
   <si>
@@ -230,6 +227,21 @@
   </si>
   <si>
     <t>Design login page</t>
+  </si>
+  <si>
+    <t>Pranay, Sonali</t>
+  </si>
+  <si>
+    <t>prof want to do items</t>
+  </si>
+  <si>
+    <t>rafir and prateek what?</t>
+  </si>
+  <si>
+    <t>API for All issues(Feed)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sonali </t>
   </si>
 </sst>
 </file>
@@ -417,7 +429,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -482,6 +494,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -941,21 +960,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.1640625" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.08203125" customWidth="1"/>
+    <col min="1" max="1" width="12.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.19921875" customWidth="1"/>
+    <col min="3" max="3" width="14.296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -969,7 +988,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="13">
         <v>1</v>
       </c>
@@ -983,7 +1002,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="13">
         <v>2</v>
       </c>
@@ -997,7 +1016,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>3</v>
       </c>
@@ -1011,7 +1030,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>4</v>
       </c>
@@ -1025,12 +1044,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>5</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>50</v>
@@ -1039,7 +1058,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>6</v>
       </c>
@@ -1053,7 +1072,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>7</v>
       </c>
@@ -1067,7 +1086,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>8</v>
       </c>
@@ -1081,7 +1100,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="14">
         <v>9</v>
       </c>
@@ -1095,7 +1114,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <v>10</v>
       </c>
@@ -1109,7 +1128,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
         <v>11</v>
       </c>
@@ -1123,7 +1142,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
         <v>12</v>
       </c>
@@ -1137,7 +1156,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>13</v>
       </c>
@@ -1151,7 +1170,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>14</v>
       </c>
@@ -1165,7 +1184,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
         <v>15</v>
       </c>
@@ -1179,7 +1198,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
         <v>16</v>
       </c>
@@ -1193,7 +1212,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="12">
         <v>17</v>
       </c>
@@ -1207,7 +1226,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="12">
         <v>18</v>
       </c>
@@ -1221,7 +1240,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
         <v>19</v>
       </c>
@@ -1235,7 +1254,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="12">
         <v>20</v>
       </c>
@@ -1249,7 +1268,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="12">
         <v>21</v>
       </c>
@@ -1263,7 +1282,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="12">
         <v>22</v>
       </c>
@@ -1277,7 +1296,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="12">
         <v>23</v>
       </c>
@@ -1291,7 +1310,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="12">
         <v>24</v>
       </c>
@@ -1305,7 +1324,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="12">
         <v>25</v>
       </c>
@@ -1319,7 +1338,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="12">
         <v>26</v>
       </c>
@@ -1333,7 +1352,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="12">
         <v>27</v>
       </c>
@@ -1347,7 +1366,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="12">
         <v>28</v>
       </c>
@@ -1361,7 +1380,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="12">
         <v>29</v>
       </c>
@@ -1375,7 +1394,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="12">
         <v>30</v>
       </c>
@@ -1389,7 +1408,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="12">
         <v>31</v>
       </c>
@@ -1403,12 +1422,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="12">
         <v>32</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C33" s="10" t="s">
         <v>49</v>
@@ -1417,12 +1436,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="12">
         <v>33</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C34" s="10" t="s">
         <v>49</v>
@@ -1431,12 +1450,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A35" s="12">
         <v>34</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C35" s="10" t="s">
         <v>49</v>
@@ -1445,31 +1464,45 @@
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A36" s="12">
         <v>35</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D36" s="12" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A37" s="12">
         <v>36</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D37" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.35">
+      <c r="A38" s="21">
+        <v>37</v>
+      </c>
+      <c r="B38" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C38" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="D38" s="21" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1482,22 +1515,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.58203125" customWidth="1"/>
-    <col min="2" max="2" width="47.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.75" customWidth="1"/>
+    <col min="1" max="1" width="12.59765625" customWidth="1"/>
+    <col min="2" max="2" width="47.296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.69921875" customWidth="1"/>
+    <col min="4" max="4" width="12.69921875" customWidth="1"/>
     <col min="5" max="5" width="38.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="23" customFormat="1" ht="21" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" s="23" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1514,7 +1547,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -1529,7 +1562,7 @@
       </c>
       <c r="E2" s="25"/>
     </row>
-    <row r="3" spans="1:5" ht="19" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -1540,11 +1573,11 @@
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="E3" s="25"/>
     </row>
-    <row r="4" spans="1:5" ht="19" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -1559,7 +1592,7 @@
       </c>
       <c r="E4" s="25"/>
     </row>
-    <row r="5" spans="1:5" ht="19" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -1574,7 +1607,7 @@
       </c>
       <c r="E5" s="25"/>
     </row>
-    <row r="6" spans="1:5" ht="19" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -1589,7 +1622,7 @@
       </c>
       <c r="E6" s="25"/>
     </row>
-    <row r="7" spans="1:5" ht="19" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -1604,7 +1637,7 @@
       </c>
       <c r="E7" s="25"/>
     </row>
-    <row r="8" spans="1:5" ht="19" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -1619,7 +1652,7 @@
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" ht="19" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -1634,7 +1667,7 @@
       </c>
       <c r="E9" s="25"/>
     </row>
-    <row r="10" spans="1:5" ht="19" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -1649,7 +1682,7 @@
       </c>
       <c r="E10" s="25"/>
     </row>
-    <row r="11" spans="1:5" ht="19" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -1664,7 +1697,7 @@
       </c>
       <c r="E11" s="25"/>
     </row>
-    <row r="12" spans="1:5" ht="19" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1679,7 +1712,7 @@
       </c>
       <c r="E12" s="25"/>
     </row>
-    <row r="13" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" ht="55.8" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1696,7 +1729,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="38" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" ht="37.200000000000003" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1713,7 +1746,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="38" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" ht="37.200000000000003" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1730,12 +1763,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="19" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.35">
       <c r="A16" s="24">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>49</v>
@@ -1745,12 +1778,12 @@
       </c>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="1:5" ht="19" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.35">
       <c r="A17" s="24">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>49</v>
@@ -1760,12 +1793,12 @@
       </c>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:5" ht="38" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" ht="37.200000000000003" x14ac:dyDescent="0.35">
       <c r="A18" s="24">
         <v>17</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>49</v>
@@ -1775,35 +1808,60 @@
       </c>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" ht="37.200000000000003" x14ac:dyDescent="0.35">
       <c r="A19" s="24">
         <v>18</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>51</v>
       </c>
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" ht="37.200000000000003" x14ac:dyDescent="0.35">
       <c r="A20" s="24">
         <v>19</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>51</v>
       </c>
       <c r="E20" s="5"/>
+    </row>
+    <row r="21" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.35">
+      <c r="A21" s="24">
+        <v>20</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="27"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>60</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1816,7 +1874,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>